<commit_message>
Complexified Model (added CAPM)
</commit_message>
<xml_diff>
--- a/phase_4_dcf_model/watchlist.xlsx
+++ b/phase_4_dcf_model/watchlist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\delic\OneDrive\Desktop\pythonvaluationmodel\phase_4_dcf_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79EF904F-571F-4A58-8F8B-2A716CD3DBD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{431D3E21-814F-465E-8F5D-281794379C1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="14860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,42 +36,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>aapl</t>
-  </si>
-  <si>
-    <t>ko</t>
-  </si>
-  <si>
-    <t>googl</t>
-  </si>
-  <si>
-    <t>nvda</t>
-  </si>
-  <si>
-    <t>tsm</t>
-  </si>
-  <si>
-    <t>pltr</t>
-  </si>
-  <si>
-    <t>amd</t>
-  </si>
-  <si>
-    <t>t</t>
-  </si>
-  <si>
-    <t>v</t>
-  </si>
-  <si>
-    <t>amzn</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>ma</t>
   </si>
 </sst>
 </file>
@@ -389,10 +356,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -402,61 +369,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated some calculations, moved to a beta version where calculations will be tested and fine tuned will revert to alpha and apply new changes once testing is complete and DCF is in line with analyst standards
</commit_message>
<xml_diff>
--- a/phase_4_dcf_model/watchlist.xlsx
+++ b/phase_4_dcf_model/watchlist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\delic\OneDrive\Desktop\pythonvaluationmodel\phase_4_dcf_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{431D3E21-814F-465E-8F5D-281794379C1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22F416BD-52F8-4378-99A2-D7B879E79608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="14860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>aapl</t>
+    <t>wmt</t>
   </si>
 </sst>
 </file>
@@ -359,7 +359,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
updated calculations, working on data import
</commit_message>
<xml_diff>
--- a/phase_4_dcf_model/watchlist.xlsx
+++ b/phase_4_dcf_model/watchlist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\delic\OneDrive\Desktop\pythonvaluationmodel\phase_4_dcf_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22F416BD-52F8-4378-99A2-D7B879E79608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD0FC65-2A0E-42F0-9232-1929245F48E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="14860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>wmt</t>
+    <t>pltr</t>
   </si>
 </sst>
 </file>
@@ -359,7 +359,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>